<commit_message>
add reactions for VEGF-B and PlGF
</commit_message>
<xml_diff>
--- a/data/reaction.xlsx
+++ b/data/reaction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunjeong/Documents/repos/x-family_membrane/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D144F8-13A6-FD42-B009-64D3EB9CBE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD026D3-2145-E24E-A62D-B399DDF0E129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22400" windowHeight="22760" xr2:uid="{1DDADA62-5B3E-DA49-9563-F9528F6ABD75}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Reaction</t>
   </si>
@@ -207,6 +207,48 @@
   </si>
   <si>
     <t>koffR1N1</t>
+  </si>
+  <si>
+    <t>VEGF-B</t>
+  </si>
+  <si>
+    <t>PlGF</t>
+  </si>
+  <si>
+    <t>VB + R1 &lt;-&gt; VB:R1</t>
+  </si>
+  <si>
+    <t>VB + N1 &lt;-&gt; VB:N1</t>
+  </si>
+  <si>
+    <t>Pl + R1 &lt;-&gt; Pl:R1</t>
+  </si>
+  <si>
+    <t>Pl + N1 &lt;-&gt; Pl:N1</t>
+  </si>
+  <si>
+    <t>konVBR1</t>
+  </si>
+  <si>
+    <t>konVBN1</t>
+  </si>
+  <si>
+    <t>koffVBR1</t>
+  </si>
+  <si>
+    <t>koffVBN1</t>
+  </si>
+  <si>
+    <t>konPlR1</t>
+  </si>
+  <si>
+    <t>koffPlR1</t>
+  </si>
+  <si>
+    <t>konPlN1</t>
+  </si>
+  <si>
+    <t>koffPlN1</t>
   </si>
 </sst>
 </file>
@@ -768,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6625652-F584-3643-A432-B66AAA5950FB}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,128 +922,186 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="A16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="A19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>